<commit_message>
Update barcode generation to ensure it never starts with zero and improve formatting
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D38B3-39CC-3440-96A9-C47229F0B9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3723E9B5-FBEF-E44B-97F6-F6BE914AF39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{1FE25D93-F9B9-E047-A2D7-4F7D4FBF066D}"/>
   </bookViews>
@@ -880,7 +880,7 @@
   <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update product name field in label generation and add new Excel file
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3723E9B5-FBEF-E44B-97F6-F6BE914AF39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073EAA1A-4966-074B-8E54-BEB979AD109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{1FE25D93-F9B9-E047-A2D7-4F7D4FBF066D}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1FE25D93-F9B9-E047-A2D7-4F7D4FBF066D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -458,10 +458,10 @@
     <t xml:space="preserve">Jean Renata Verde Menta Petite Cadera </t>
   </si>
   <si>
-    <t>Nombre Etiqueta (quitar para bsale)</t>
-  </si>
-  <si>
-    <t>Descripción (nombre producto/servicio)</t>
+    <t>Nombre Producto/Servicio</t>
+  </si>
+  <si>
+    <t>Nombre Etiqueta</t>
   </si>
 </sst>
 </file>
@@ -503,15 +503,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -539,8 +531,8 @@
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{10B309C5-388F-904C-9561-58B202696661}" name="Clasificación" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{CC319B42-768D-4D42-A497-7B5AF8017B6D}" name="Tipo de producto o servicio" dataCellStyle="Normal"/>
-    <tableColumn id="18" xr3:uid="{A708F923-FA32-6941-8071-8F7CAECCCE44}" name="Descripción (nombre producto/servicio)"/>
-    <tableColumn id="3" xr3:uid="{1F4C2C15-FB0C-7240-8509-78238EEE041A}" name="Nombre Etiqueta (quitar para bsale)" dataCellStyle="Normal"/>
+    <tableColumn id="18" xr3:uid="{A708F923-FA32-6941-8071-8F7CAECCCE44}" name="Nombre Producto/Servicio"/>
+    <tableColumn id="3" xr3:uid="{1F4C2C15-FB0C-7240-8509-78238EEE041A}" name="Nombre Etiqueta" dataCellStyle="Normal"/>
     <tableColumn id="4" xr3:uid="{6C128F37-F492-0D47-B5A5-07EBF1C7F592}" name="Variante" dataCellStyle="Normal"/>
     <tableColumn id="17" xr3:uid="{0CE2199F-302C-BE43-A94C-F1977E4F11BB}" name="Tamanio"/>
     <tableColumn id="16" xr3:uid="{978016AA-EE75-7948-9E8C-511B95AE98A9}" name="Posicion"/>
@@ -880,14 +872,14 @@
   <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" customWidth="1"/>
@@ -905,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
         <v>141</v>
-      </c>
-      <c r="D1" t="s">
-        <v>140</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1010,6 +1002,10 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
+      <c r="C3" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Verde Menta Petite Cadera</v>
+      </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
@@ -1057,6 +1053,10 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
+      <c r="C4" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Verde Menta Petite Cadera</v>
+      </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1104,6 +1104,10 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Verde Menta Petite Cadera</v>
+      </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -1151,6 +1155,10 @@
       <c r="B6" t="s">
         <v>17</v>
       </c>
+      <c r="C6" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Verde Menta Petite Cadera</v>
+      </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
@@ -1198,6 +1206,10 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="C7" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Militar Petite Cadera</v>
+      </c>
       <c r="D7" t="s">
         <v>35</v>
       </c>
@@ -1245,6 +1257,10 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
+      <c r="C8" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Militar Petite Cadera</v>
+      </c>
       <c r="D8" t="s">
         <v>35</v>
       </c>
@@ -1292,6 +1308,10 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Militar Petite Cadera</v>
+      </c>
       <c r="D9" t="s">
         <v>35</v>
       </c>
@@ -1339,6 +1359,10 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Militar Petite Cadera</v>
+      </c>
       <c r="D10" t="s">
         <v>35</v>
       </c>
@@ -1386,6 +1410,10 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Militar Petite Cadera</v>
+      </c>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -1433,6 +1461,10 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Marfil Petite Cadera</v>
+      </c>
       <c r="D12" t="s">
         <v>41</v>
       </c>
@@ -1480,6 +1512,10 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Marfil Petite Cadera</v>
+      </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -1527,6 +1563,10 @@
       <c r="B14" t="s">
         <v>17</v>
       </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Marfil Petite Cadera</v>
+      </c>
       <c r="D14" t="s">
         <v>41</v>
       </c>
@@ -1574,6 +1614,10 @@
       <c r="B15" t="s">
         <v>17</v>
       </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Marfil Petite Cadera</v>
+      </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
@@ -1621,6 +1665,10 @@
       <c r="B16" t="s">
         <v>17</v>
       </c>
+      <c r="C16" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Marfil Petite Cadera</v>
+      </c>
       <c r="D16" t="s">
         <v>41</v>
       </c>
@@ -1668,6 +1716,10 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
+      <c r="C17" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Negro Petite Cadera</v>
+      </c>
       <c r="D17" t="s">
         <v>47</v>
       </c>
@@ -1715,6 +1767,10 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
+      <c r="C18" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Negro Petite Cadera</v>
+      </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
@@ -1762,6 +1818,10 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
+      <c r="C19" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Negro Petite Cadera</v>
+      </c>
       <c r="D19" t="s">
         <v>47</v>
       </c>
@@ -1809,6 +1869,10 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
+      <c r="C20" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Negro Petite Cadera</v>
+      </c>
       <c r="D20" t="s">
         <v>47</v>
       </c>
@@ -1856,6 +1920,10 @@
       <c r="B21" t="s">
         <v>17</v>
       </c>
+      <c r="C21" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Negro Petite Cadera</v>
+      </c>
       <c r="D21" t="s">
         <v>47</v>
       </c>
@@ -1903,6 +1971,10 @@
       <c r="B22" t="s">
         <v>17</v>
       </c>
+      <c r="C22" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Lila Petite Cadera</v>
+      </c>
       <c r="D22" t="s">
         <v>53</v>
       </c>
@@ -1950,6 +2022,10 @@
       <c r="B23" t="s">
         <v>17</v>
       </c>
+      <c r="C23" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Lila Petite Cadera</v>
+      </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
@@ -1997,6 +2073,10 @@
       <c r="B24" t="s">
         <v>17</v>
       </c>
+      <c r="C24" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Lila Petite Cadera</v>
+      </c>
       <c r="D24" t="s">
         <v>53</v>
       </c>
@@ -2044,6 +2124,10 @@
       <c r="B25" t="s">
         <v>17</v>
       </c>
+      <c r="C25" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Lila Petite Cadera</v>
+      </c>
       <c r="D25" t="s">
         <v>53</v>
       </c>
@@ -2091,6 +2175,10 @@
       <c r="B26" t="s">
         <v>17</v>
       </c>
+      <c r="C26" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Lila Petite Cadera</v>
+      </c>
       <c r="D26" t="s">
         <v>53</v>
       </c>
@@ -2138,6 +2226,10 @@
       <c r="B27" t="s">
         <v>17</v>
       </c>
+      <c r="C27" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Habano Petite Cadera</v>
+      </c>
       <c r="D27" t="s">
         <v>60</v>
       </c>
@@ -2185,6 +2277,10 @@
       <c r="B28" t="s">
         <v>17</v>
       </c>
+      <c r="C28" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Habano Petite Cadera</v>
+      </c>
       <c r="D28" t="s">
         <v>60</v>
       </c>
@@ -2232,6 +2328,10 @@
       <c r="B29" t="s">
         <v>17</v>
       </c>
+      <c r="C29" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Habano Petite Cadera</v>
+      </c>
       <c r="D29" t="s">
         <v>60</v>
       </c>
@@ -2279,6 +2379,10 @@
       <c r="B30" t="s">
         <v>17</v>
       </c>
+      <c r="C30" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Habano Petite Cadera</v>
+      </c>
       <c r="D30" t="s">
         <v>60</v>
       </c>
@@ -2326,6 +2430,10 @@
       <c r="B31" t="s">
         <v>17</v>
       </c>
+      <c r="C31" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Renata Habano Petite Cadera</v>
+      </c>
       <c r="D31" t="s">
         <v>60</v>
       </c>
@@ -2373,6 +2481,10 @@
       <c r="B32" t="s">
         <v>17</v>
       </c>
+      <c r="C32" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Regular Cadera</v>
+      </c>
       <c r="D32" t="s">
         <v>66</v>
       </c>
@@ -2420,6 +2532,10 @@
       <c r="B33" t="s">
         <v>17</v>
       </c>
+      <c r="C33" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Regular Cadera</v>
+      </c>
       <c r="D33" t="s">
         <v>66</v>
       </c>
@@ -2467,6 +2583,10 @@
       <c r="B34" t="s">
         <v>17</v>
       </c>
+      <c r="C34" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Regular Cadera</v>
+      </c>
       <c r="D34" t="s">
         <v>66</v>
       </c>
@@ -2514,6 +2634,10 @@
       <c r="B35" t="s">
         <v>17</v>
       </c>
+      <c r="C35" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Regular Cadera</v>
+      </c>
       <c r="D35" t="s">
         <v>66</v>
       </c>
@@ -2561,6 +2685,10 @@
       <c r="B36" t="s">
         <v>17</v>
       </c>
+      <c r="C36" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Regular Cadera</v>
+      </c>
       <c r="D36" t="s">
         <v>66</v>
       </c>
@@ -2608,6 +2736,10 @@
       <c r="B37" t="s">
         <v>17</v>
       </c>
+      <c r="C37" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Regular Cadera</v>
+      </c>
       <c r="D37" t="s">
         <v>72</v>
       </c>
@@ -2655,6 +2787,10 @@
       <c r="B38" t="s">
         <v>17</v>
       </c>
+      <c r="C38" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Regular Cadera</v>
+      </c>
       <c r="D38" t="s">
         <v>72</v>
       </c>
@@ -2702,6 +2838,10 @@
       <c r="B39" t="s">
         <v>17</v>
       </c>
+      <c r="C39" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Regular Cadera</v>
+      </c>
       <c r="D39" t="s">
         <v>72</v>
       </c>
@@ -2749,6 +2889,10 @@
       <c r="B40" t="s">
         <v>17</v>
       </c>
+      <c r="C40" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Regular Cadera</v>
+      </c>
       <c r="D40" t="s">
         <v>72</v>
       </c>
@@ -2796,6 +2940,10 @@
       <c r="B41" t="s">
         <v>17</v>
       </c>
+      <c r="C41" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Regular Cadera</v>
+      </c>
       <c r="D41" t="s">
         <v>72</v>
       </c>
@@ -2843,6 +2991,10 @@
       <c r="B42" t="s">
         <v>17</v>
       </c>
+      <c r="C42" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Regular Cadera</v>
+      </c>
       <c r="D42" t="s">
         <v>78</v>
       </c>
@@ -2890,6 +3042,10 @@
       <c r="B43" t="s">
         <v>17</v>
       </c>
+      <c r="C43" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Regular Cadera</v>
+      </c>
       <c r="D43" t="s">
         <v>78</v>
       </c>
@@ -2937,6 +3093,10 @@
       <c r="B44" t="s">
         <v>17</v>
       </c>
+      <c r="C44" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Regular Cadera</v>
+      </c>
       <c r="D44" t="s">
         <v>78</v>
       </c>
@@ -2984,6 +3144,10 @@
       <c r="B45" t="s">
         <v>17</v>
       </c>
+      <c r="C45" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Regular Cadera</v>
+      </c>
       <c r="D45" t="s">
         <v>78</v>
       </c>
@@ -3031,6 +3195,10 @@
       <c r="B46" t="s">
         <v>17</v>
       </c>
+      <c r="C46" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Regular Cadera</v>
+      </c>
       <c r="D46" t="s">
         <v>78</v>
       </c>
@@ -3078,6 +3246,10 @@
       <c r="B47" t="s">
         <v>17</v>
       </c>
+      <c r="C47" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Regular Cadera</v>
+      </c>
       <c r="D47" t="s">
         <v>84</v>
       </c>
@@ -3125,6 +3297,10 @@
       <c r="B48" t="s">
         <v>17</v>
       </c>
+      <c r="C48" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Regular Cadera</v>
+      </c>
       <c r="D48" t="s">
         <v>84</v>
       </c>
@@ -3172,6 +3348,10 @@
       <c r="B49" t="s">
         <v>17</v>
       </c>
+      <c r="C49" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Regular Cadera</v>
+      </c>
       <c r="D49" t="s">
         <v>84</v>
       </c>
@@ -3219,6 +3399,10 @@
       <c r="B50" t="s">
         <v>17</v>
       </c>
+      <c r="C50" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Regular Cadera</v>
+      </c>
       <c r="D50" t="s">
         <v>84</v>
       </c>
@@ -3266,6 +3450,10 @@
       <c r="B51" t="s">
         <v>17</v>
       </c>
+      <c r="C51" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Regular Cadera</v>
+      </c>
       <c r="D51" t="s">
         <v>84</v>
       </c>
@@ -3313,6 +3501,10 @@
       <c r="B52" t="s">
         <v>17</v>
       </c>
+      <c r="C52" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Regular Cadera</v>
+      </c>
       <c r="D52" t="s">
         <v>90</v>
       </c>
@@ -3360,6 +3552,10 @@
       <c r="B53" t="s">
         <v>17</v>
       </c>
+      <c r="C53" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Regular Cadera</v>
+      </c>
       <c r="D53" t="s">
         <v>90</v>
       </c>
@@ -3407,6 +3603,10 @@
       <c r="B54" t="s">
         <v>17</v>
       </c>
+      <c r="C54" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Regular Cadera</v>
+      </c>
       <c r="D54" t="s">
         <v>90</v>
       </c>
@@ -3454,6 +3654,10 @@
       <c r="B55" t="s">
         <v>17</v>
       </c>
+      <c r="C55" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Regular Cadera</v>
+      </c>
       <c r="D55" t="s">
         <v>90</v>
       </c>
@@ -3501,6 +3705,10 @@
       <c r="B56" t="s">
         <v>17</v>
       </c>
+      <c r="C56" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Regular Cadera</v>
+      </c>
       <c r="D56" t="s">
         <v>90</v>
       </c>
@@ -3548,6 +3756,10 @@
       <c r="B57" t="s">
         <v>17</v>
       </c>
+      <c r="C57" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Blue Wash Petite Cadera</v>
+      </c>
       <c r="D57" t="s">
         <v>96</v>
       </c>
@@ -3595,6 +3807,10 @@
       <c r="B58" t="s">
         <v>17</v>
       </c>
+      <c r="C58" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Blue Wash Petite Cadera</v>
+      </c>
       <c r="D58" t="s">
         <v>96</v>
       </c>
@@ -3642,6 +3858,10 @@
       <c r="B59" t="s">
         <v>17</v>
       </c>
+      <c r="C59" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Blue Wash Petite Cadera</v>
+      </c>
       <c r="D59" t="s">
         <v>96</v>
       </c>
@@ -3689,6 +3909,10 @@
       <c r="B60" t="s">
         <v>17</v>
       </c>
+      <c r="C60" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Blue Wash Petite Cadera</v>
+      </c>
       <c r="D60" t="s">
         <v>96</v>
       </c>
@@ -3736,6 +3960,10 @@
       <c r="B61" t="s">
         <v>17</v>
       </c>
+      <c r="C61" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Blue Wash Petite Cadera</v>
+      </c>
       <c r="D61" t="s">
         <v>96</v>
       </c>
@@ -3783,6 +4011,10 @@
       <c r="B62" t="s">
         <v>17</v>
       </c>
+      <c r="C62" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Corn Wash Petite Cadera</v>
+      </c>
       <c r="D62" t="s">
         <v>102</v>
       </c>
@@ -3830,6 +4062,10 @@
       <c r="B63" t="s">
         <v>17</v>
       </c>
+      <c r="C63" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Corn Wash Petite Cadera</v>
+      </c>
       <c r="D63" t="s">
         <v>102</v>
       </c>
@@ -3877,6 +4113,10 @@
       <c r="B64" t="s">
         <v>17</v>
       </c>
+      <c r="C64" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Corn Wash Petite Cadera</v>
+      </c>
       <c r="D64" t="s">
         <v>102</v>
       </c>
@@ -3924,6 +4164,10 @@
       <c r="B65" t="s">
         <v>17</v>
       </c>
+      <c r="C65" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Corn Wash Petite Cadera</v>
+      </c>
       <c r="D65" t="s">
         <v>102</v>
       </c>
@@ -3971,6 +4215,10 @@
       <c r="B66" t="s">
         <v>17</v>
       </c>
+      <c r="C66" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Corn Wash Petite Cadera</v>
+      </c>
       <c r="D66" t="s">
         <v>102</v>
       </c>
@@ -4018,6 +4266,10 @@
       <c r="B67" t="s">
         <v>17</v>
       </c>
+      <c r="C67" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Ice Wash Petite Cadera</v>
+      </c>
       <c r="D67" t="s">
         <v>108</v>
       </c>
@@ -4065,6 +4317,10 @@
       <c r="B68" t="s">
         <v>17</v>
       </c>
+      <c r="C68" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Ice Wash Petite Cadera</v>
+      </c>
       <c r="D68" t="s">
         <v>108</v>
       </c>
@@ -4112,6 +4368,10 @@
       <c r="B69" t="s">
         <v>17</v>
       </c>
+      <c r="C69" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Ice Wash Petite Cadera</v>
+      </c>
       <c r="D69" t="s">
         <v>108</v>
       </c>
@@ -4159,6 +4419,10 @@
       <c r="B70" t="s">
         <v>17</v>
       </c>
+      <c r="C70" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Ice Wash Petite Cadera</v>
+      </c>
       <c r="D70" t="s">
         <v>108</v>
       </c>
@@ -4206,6 +4470,10 @@
       <c r="B71" t="s">
         <v>17</v>
       </c>
+      <c r="C71" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Sohana Ice Wash Petite Cadera</v>
+      </c>
       <c r="D71" t="s">
         <v>108</v>
       </c>
@@ -4253,6 +4521,10 @@
       <c r="B72" t="s">
         <v>17</v>
       </c>
+      <c r="C72" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Petite Cadera</v>
+      </c>
       <c r="D72" t="s">
         <v>66</v>
       </c>
@@ -4300,6 +4572,10 @@
       <c r="B73" t="s">
         <v>17</v>
       </c>
+      <c r="C73" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Petite Cadera</v>
+      </c>
       <c r="D73" t="s">
         <v>66</v>
       </c>
@@ -4347,6 +4623,10 @@
       <c r="B74" t="s">
         <v>17</v>
       </c>
+      <c r="C74" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Petite Cadera</v>
+      </c>
       <c r="D74" t="s">
         <v>66</v>
       </c>
@@ -4394,6 +4674,10 @@
       <c r="B75" t="s">
         <v>17</v>
       </c>
+      <c r="C75" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Petite Cadera</v>
+      </c>
       <c r="D75" t="s">
         <v>66</v>
       </c>
@@ -4441,6 +4725,10 @@
       <c r="B76" t="s">
         <v>17</v>
       </c>
+      <c r="C76" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Acid Wash Petite Cadera</v>
+      </c>
       <c r="D76" t="s">
         <v>66</v>
       </c>
@@ -4488,6 +4776,10 @@
       <c r="B77" t="s">
         <v>17</v>
       </c>
+      <c r="C77" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Petite Cadera</v>
+      </c>
       <c r="D77" t="s">
         <v>72</v>
       </c>
@@ -4535,6 +4827,10 @@
       <c r="B78" t="s">
         <v>17</v>
       </c>
+      <c r="C78" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Petite Cadera</v>
+      </c>
       <c r="D78" t="s">
         <v>72</v>
       </c>
@@ -4582,6 +4878,10 @@
       <c r="B79" t="s">
         <v>17</v>
       </c>
+      <c r="C79" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Petite Cadera</v>
+      </c>
       <c r="D79" t="s">
         <v>72</v>
       </c>
@@ -4629,6 +4929,10 @@
       <c r="B80" t="s">
         <v>17</v>
       </c>
+      <c r="C80" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Petite Cadera</v>
+      </c>
       <c r="D80" t="s">
         <v>72</v>
       </c>
@@ -4676,6 +4980,10 @@
       <c r="B81" t="s">
         <v>17</v>
       </c>
+      <c r="C81" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Grenish Blue Petite Cadera</v>
+      </c>
       <c r="D81" t="s">
         <v>72</v>
       </c>
@@ -4723,6 +5031,10 @@
       <c r="B82" t="s">
         <v>17</v>
       </c>
+      <c r="C82" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Petite Cadera</v>
+      </c>
       <c r="D82" t="s">
         <v>78</v>
       </c>
@@ -4770,6 +5082,10 @@
       <c r="B83" t="s">
         <v>17</v>
       </c>
+      <c r="C83" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Petite Cadera</v>
+      </c>
       <c r="D83" t="s">
         <v>78</v>
       </c>
@@ -4817,6 +5133,10 @@
       <c r="B84" t="s">
         <v>17</v>
       </c>
+      <c r="C84" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Petite Cadera</v>
+      </c>
       <c r="D84" t="s">
         <v>78</v>
       </c>
@@ -4864,6 +5184,10 @@
       <c r="B85" t="s">
         <v>17</v>
       </c>
+      <c r="C85" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Petite Cadera</v>
+      </c>
       <c r="D85" t="s">
         <v>78</v>
       </c>
@@ -4911,6 +5235,10 @@
       <c r="B86" t="s">
         <v>17</v>
       </c>
+      <c r="C86" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Corn Wash Petite Cadera</v>
+      </c>
       <c r="D86" t="s">
         <v>78</v>
       </c>
@@ -4958,6 +5286,10 @@
       <c r="B87" t="s">
         <v>17</v>
       </c>
+      <c r="C87" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Petite Cadera</v>
+      </c>
       <c r="D87" t="s">
         <v>84</v>
       </c>
@@ -5005,6 +5337,10 @@
       <c r="B88" t="s">
         <v>17</v>
       </c>
+      <c r="C88" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Petite Cadera</v>
+      </c>
       <c r="D88" t="s">
         <v>84</v>
       </c>
@@ -5052,6 +5388,10 @@
       <c r="B89" t="s">
         <v>17</v>
       </c>
+      <c r="C89" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Petite Cadera</v>
+      </c>
       <c r="D89" t="s">
         <v>84</v>
       </c>
@@ -5099,6 +5439,10 @@
       <c r="B90" t="s">
         <v>17</v>
       </c>
+      <c r="C90" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Petite Cadera</v>
+      </c>
       <c r="D90" t="s">
         <v>84</v>
       </c>
@@ -5146,6 +5490,10 @@
       <c r="B91" t="s">
         <v>17</v>
       </c>
+      <c r="C91" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Sky Blue Petite Cadera</v>
+      </c>
       <c r="D91" t="s">
         <v>84</v>
       </c>
@@ -5193,6 +5541,10 @@
       <c r="B92" t="s">
         <v>17</v>
       </c>
+      <c r="C92" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Petite Cadera</v>
+      </c>
       <c r="D92" t="s">
         <v>90</v>
       </c>
@@ -5240,6 +5592,10 @@
       <c r="B93" t="s">
         <v>17</v>
       </c>
+      <c r="C93" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Petite Cadera</v>
+      </c>
       <c r="D93" t="s">
         <v>90</v>
       </c>
@@ -5287,6 +5643,10 @@
       <c r="B94" t="s">
         <v>17</v>
       </c>
+      <c r="C94" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Petite Cadera</v>
+      </c>
       <c r="D94" t="s">
         <v>90</v>
       </c>
@@ -5334,6 +5694,10 @@
       <c r="B95" t="s">
         <v>17</v>
       </c>
+      <c r="C95" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Petite Cadera</v>
+      </c>
       <c r="D95" t="s">
         <v>90</v>
       </c>
@@ -5380,6 +5744,10 @@
       </c>
       <c r="B96" t="s">
         <v>17</v>
+      </c>
+      <c r="C96" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Nombre Etiqueta]]," ",Tabla1[[#This Row],[Tamanio]]," ",Tabla1[[#This Row],[Posicion]])</f>
+        <v>Jean Ballion Brown Wash Petite Cadera</v>
       </c>
       <c r="D96" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Add new Excel file for fifth delivery of product codes
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6A9183-BD21-6F46-A30E-3970C3E976D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E4555E-FA62-934F-A4D9-1D3C4ABBAF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="U13" sqref="A1:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add new Excel file with product codes and details for 2025-08-29
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB45A0BD-87AC-E14B-B805-F269D0244CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B35C63-7F18-3743-828E-A28A146CA1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="69">
   <si>
     <t>Clasificación</t>
   </si>
@@ -101,40 +88,145 @@
     <t>Producto</t>
   </si>
   <si>
+    <t>Jeans </t>
+  </si>
+  <si>
+    <t>Jean Baggy Dennis Reg, Cint. Ice Wash</t>
+  </si>
+  <si>
+    <t>Dennis Ice Wash</t>
+  </si>
+  <si>
+    <t>Talla 26</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Baggy</t>
+  </si>
+  <si>
+    <t>Ice Wash</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Cintura</t>
+  </si>
+  <si>
+    <t>JOLG</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-IW-26</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Jean Baggy Dennis Reg. Cint. Ice Wash</t>
+  </si>
+  <si>
+    <t>Talla 28</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-IW-28</t>
+  </si>
+  <si>
+    <t>Talla 30</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-IW-30</t>
+  </si>
+  <si>
+    <t>Talla 32</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-IW-32</t>
+  </si>
+  <si>
+    <t>Talla 34</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-IW-34</t>
+  </si>
+  <si>
+    <t>Jean Baggy Dennis Reg. Cint. Sky Blue</t>
+  </si>
+  <si>
+    <t>Dennis Sky Blue</t>
+  </si>
+  <si>
     <t>Sky Blue</t>
   </si>
   <si>
-    <t>JOLG</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>Jeans </t>
-  </si>
-  <si>
-    <t>Ballion Sky Blue</t>
-  </si>
-  <si>
-    <t>Jean Ballion Petite Cadera Sky Blue</t>
-  </si>
-  <si>
-    <t>Talla 26</t>
-  </si>
-  <si>
-    <t>Petite</t>
-  </si>
-  <si>
-    <t>Ballion</t>
-  </si>
-  <si>
-    <t>Cadera</t>
-  </si>
-  <si>
-    <t>52501-P-SB26</t>
+    <t>52505-JEAN-DEN-SB-26</t>
+  </si>
+  <si>
+    <t>Jean BaggyDennis Reg. Cint. Sky Blue</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-SB-28</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-SB-30</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-SB-32</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-SB-34</t>
+  </si>
+  <si>
+    <t>Jean Baggy Dennis Reg. Cint. Wood Blue</t>
+  </si>
+  <si>
+    <t>Dennis Wood Blue</t>
+  </si>
+  <si>
+    <t>Wood Blue</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-WB-26</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-WB-28</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-WB-30</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-WB-32</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-WB-34</t>
+  </si>
+  <si>
+    <t>Jean Baggy Dennis Reg. Cint. Acid Wash</t>
+  </si>
+  <si>
+    <t>Dennis Acid Wash</t>
+  </si>
+  <si>
+    <t>Acid Wash</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-AW-26</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-AW-28</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-AW-30</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-AW-32</t>
+  </si>
+  <si>
+    <t>52505-JEAN-DEN-AW-34</t>
   </si>
 </sst>
 </file>
@@ -153,7 +245,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,11 +282,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,20 +590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -584,46 +671,49 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2">
-        <v>701938229777</v>
+      <c r="M2" s="2">
+        <v>602783942271</v>
       </c>
       <c r="N2" t="s">
         <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="P2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R2">
         <v>100</v>
@@ -635,7 +725,1185 @@
         <v>95</v>
       </c>
       <c r="U2">
-        <v>115</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="2">
+        <v>603665056981</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3">
+        <v>33</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <v>75</v>
+      </c>
+      <c r="T3">
+        <v>95</v>
+      </c>
+      <c r="U3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="2">
+        <v>600792853872</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4">
+        <v>33</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4">
+        <v>75</v>
+      </c>
+      <c r="T4">
+        <v>95</v>
+      </c>
+      <c r="U4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="2">
+        <v>603234629446</v>
+      </c>
+      <c r="N5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5">
+        <v>22</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>75</v>
+      </c>
+      <c r="T5">
+        <v>95</v>
+      </c>
+      <c r="U5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="2">
+        <v>600158122850</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6">
+        <v>75</v>
+      </c>
+      <c r="T6">
+        <v>95</v>
+      </c>
+      <c r="U6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="2">
+        <v>603980425028</v>
+      </c>
+      <c r="N7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7">
+        <v>11</v>
+      </c>
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7">
+        <v>75</v>
+      </c>
+      <c r="T7">
+        <v>95</v>
+      </c>
+      <c r="U7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="2">
+        <v>603631959498</v>
+      </c>
+      <c r="N8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8">
+        <v>33</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8">
+        <v>75</v>
+      </c>
+      <c r="T8">
+        <v>95</v>
+      </c>
+      <c r="U8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="2">
+        <v>601106538064</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9">
+        <v>33</v>
+      </c>
+      <c r="R9">
+        <v>100</v>
+      </c>
+      <c r="S9">
+        <v>75</v>
+      </c>
+      <c r="T9">
+        <v>95</v>
+      </c>
+      <c r="U9">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="2">
+        <v>602843779049</v>
+      </c>
+      <c r="N10" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10">
+        <v>22</v>
+      </c>
+      <c r="R10">
+        <v>100</v>
+      </c>
+      <c r="S10">
+        <v>75</v>
+      </c>
+      <c r="T10">
+        <v>95</v>
+      </c>
+      <c r="U10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="2">
+        <v>601838378870</v>
+      </c>
+      <c r="N11" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11">
+        <v>11</v>
+      </c>
+      <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11">
+        <v>75</v>
+      </c>
+      <c r="T11">
+        <v>95</v>
+      </c>
+      <c r="U11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="2">
+        <v>602131458545</v>
+      </c>
+      <c r="N12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>100</v>
+      </c>
+      <c r="S12">
+        <v>75</v>
+      </c>
+      <c r="T12">
+        <v>95</v>
+      </c>
+      <c r="U12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="2">
+        <v>602956435585</v>
+      </c>
+      <c r="N13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13">
+        <v>33</v>
+      </c>
+      <c r="R13">
+        <v>100</v>
+      </c>
+      <c r="S13">
+        <v>75</v>
+      </c>
+      <c r="T13">
+        <v>95</v>
+      </c>
+      <c r="U13">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="2">
+        <v>601733247673</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14">
+        <v>33</v>
+      </c>
+      <c r="R14">
+        <v>100</v>
+      </c>
+      <c r="S14">
+        <v>75</v>
+      </c>
+      <c r="T14">
+        <v>95</v>
+      </c>
+      <c r="U14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="2">
+        <v>600181857375</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15">
+        <v>22</v>
+      </c>
+      <c r="R15">
+        <v>100</v>
+      </c>
+      <c r="S15">
+        <v>75</v>
+      </c>
+      <c r="T15">
+        <v>95</v>
+      </c>
+      <c r="U15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="2">
+        <v>602537391321</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16">
+        <v>11</v>
+      </c>
+      <c r="R16">
+        <v>100</v>
+      </c>
+      <c r="S16">
+        <v>75</v>
+      </c>
+      <c r="T16">
+        <v>95</v>
+      </c>
+      <c r="U16">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="2">
+        <v>604155392228</v>
+      </c>
+      <c r="N17" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17" t="s">
+        <v>34</v>
+      </c>
+      <c r="P17">
+        <v>11</v>
+      </c>
+      <c r="R17">
+        <v>100</v>
+      </c>
+      <c r="S17">
+        <v>75</v>
+      </c>
+      <c r="T17">
+        <v>95</v>
+      </c>
+      <c r="U17">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="2">
+        <v>602042358508</v>
+      </c>
+      <c r="N18" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18">
+        <v>33</v>
+      </c>
+      <c r="R18">
+        <v>100</v>
+      </c>
+      <c r="S18">
+        <v>75</v>
+      </c>
+      <c r="T18">
+        <v>95</v>
+      </c>
+      <c r="U18">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="2">
+        <v>600646159462</v>
+      </c>
+      <c r="N19" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19">
+        <v>33</v>
+      </c>
+      <c r="R19">
+        <v>100</v>
+      </c>
+      <c r="S19">
+        <v>75</v>
+      </c>
+      <c r="T19">
+        <v>95</v>
+      </c>
+      <c r="U19">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" s="2">
+        <v>600653780706</v>
+      </c>
+      <c r="N20" t="s">
+        <v>67</v>
+      </c>
+      <c r="O20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20">
+        <v>22</v>
+      </c>
+      <c r="R20">
+        <v>100</v>
+      </c>
+      <c r="S20">
+        <v>75</v>
+      </c>
+      <c r="T20">
+        <v>95</v>
+      </c>
+      <c r="U20">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="2">
+        <v>603680627959</v>
+      </c>
+      <c r="N21" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21">
+        <v>11</v>
+      </c>
+      <c r="R21">
+        <v>100</v>
+      </c>
+      <c r="S21">
+        <v>75</v>
+      </c>
+      <c r="T21">
+        <v>95</v>
+      </c>
+      <c r="U21">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Excel file for sixth delivery of product codes
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B35C63-7F18-3743-828E-A28A146CA1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC481DF4-CDB2-F64E-82DB-1A71AF28B2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,11 +593,15 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="13" max="13" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add new Excel file with product codes and details from September 2025
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC481DF4-CDB2-F64E-82DB-1A71AF28B2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E285CF49-7065-9040-BA1E-41E99854DFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="128">
   <si>
     <t>Clasificación</t>
   </si>
@@ -91,10 +104,10 @@
     <t>Jeans </t>
   </si>
   <si>
-    <t>Jean Baggy Dennis Reg, Cint. Ice Wash</t>
-  </si>
-  <si>
-    <t>Dennis Ice Wash</t>
+    <t>Ramy Reg. Cint. Negro</t>
+  </si>
+  <si>
+    <t>Flare Ramy Negro</t>
   </si>
   <si>
     <t>Talla 26</t>
@@ -103,130 +116,307 @@
     <t>Regular</t>
   </si>
   <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Negro</t>
+  </si>
+  <si>
+    <t>Ramy</t>
+  </si>
+  <si>
+    <t>Cintura</t>
+  </si>
+  <si>
+    <t>JOLG</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>602230208069</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-NE-26</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Talla 28</t>
+  </si>
+  <si>
+    <t>603113820447</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-NE-28</t>
+  </si>
+  <si>
+    <t>Talla 30</t>
+  </si>
+  <si>
+    <t>602345084894</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-NE-30</t>
+  </si>
+  <si>
+    <t>Talla 32</t>
+  </si>
+  <si>
+    <t>603602012288</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-NE-32</t>
+  </si>
+  <si>
+    <t>Talla 34</t>
+  </si>
+  <si>
+    <t>602708001816</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-NE-34</t>
+  </si>
+  <si>
+    <t>Ramy Reg. Cint. Chocolate</t>
+  </si>
+  <si>
+    <t>Flare Ramy Chocolate</t>
+  </si>
+  <si>
+    <t>603833336959</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-CH-26</t>
+  </si>
+  <si>
+    <t>602052804481</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-CH-28</t>
+  </si>
+  <si>
+    <t>602764853870</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-CH-30</t>
+  </si>
+  <si>
+    <t>600050008816</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-CH-32</t>
+  </si>
+  <si>
+    <t>603427794902</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-CH-34</t>
+  </si>
+  <si>
+    <t>Ramy Reg. Cint. Verde</t>
+  </si>
+  <si>
+    <t>Flare Ramy Verde</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>600585951612</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-VE-26</t>
+  </si>
+  <si>
+    <t>601192474129</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-VE-28</t>
+  </si>
+  <si>
+    <t>602975714184</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-VE-30</t>
+  </si>
+  <si>
+    <t>601315808447</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-VE-32</t>
+  </si>
+  <si>
+    <t>601647522641</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-VE-34</t>
+  </si>
+  <si>
+    <t>Ramy Reg. Cint. Beige</t>
+  </si>
+  <si>
+    <t>Flare Ramy Beige</t>
+  </si>
+  <si>
+    <t>Beige</t>
+  </si>
+  <si>
+    <t>603640904205</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-BE-26</t>
+  </si>
+  <si>
+    <t>601035431058</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-BE-28</t>
+  </si>
+  <si>
+    <t>602120561476</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-BE-30</t>
+  </si>
+  <si>
+    <t>602932427470</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-BE-32</t>
+  </si>
+  <si>
+    <t>601917954784</t>
+  </si>
+  <si>
+    <t>0625-JEAN-RAM-BE-34</t>
+  </si>
+  <si>
+    <t>Romina Reg. Cint. Corn Wash</t>
+  </si>
+  <si>
+    <t>Baggy Romina Corn Wash</t>
+  </si>
+  <si>
     <t>Baggy</t>
   </si>
   <si>
-    <t>Ice Wash</t>
-  </si>
-  <si>
-    <t>Dennis</t>
-  </si>
-  <si>
-    <t>Cintura</t>
-  </si>
-  <si>
-    <t>JOLG</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-IW-26</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>Jean Baggy Dennis Reg. Cint. Ice Wash</t>
-  </si>
-  <si>
-    <t>Talla 28</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-IW-28</t>
-  </si>
-  <si>
-    <t>Talla 30</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-IW-30</t>
-  </si>
-  <si>
-    <t>Talla 32</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-IW-32</t>
-  </si>
-  <si>
-    <t>Talla 34</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-IW-34</t>
-  </si>
-  <si>
-    <t>Jean Baggy Dennis Reg. Cint. Sky Blue</t>
-  </si>
-  <si>
-    <t>Dennis Sky Blue</t>
+    <t>Corn Wash</t>
+  </si>
+  <si>
+    <t>Romina</t>
+  </si>
+  <si>
+    <t>601207794463</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-CW-26</t>
+  </si>
+  <si>
+    <t>600942372705</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-CW-28</t>
+  </si>
+  <si>
+    <t>601328813338</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-CW-30</t>
+  </si>
+  <si>
+    <t>600747615074</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-CW-32</t>
+  </si>
+  <si>
+    <t>600718045196</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-CW-34</t>
+  </si>
+  <si>
+    <t>Romina Reg. Cint. Acid Wash</t>
+  </si>
+  <si>
+    <t>Baggy Romina Acid Wash</t>
+  </si>
+  <si>
+    <t>Acid Wash</t>
+  </si>
+  <si>
+    <t>602624753647</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-AW-26</t>
+  </si>
+  <si>
+    <t>603472028728</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-AW-28</t>
+  </si>
+  <si>
+    <t>602695463130</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-AW-30</t>
+  </si>
+  <si>
+    <t>602740772890</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-AW-32</t>
+  </si>
+  <si>
+    <t>602156473578</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-AW-34</t>
+  </si>
+  <si>
+    <t>Romina Reg. Cint. Sky Blue</t>
+  </si>
+  <si>
+    <t>Baggy Romina Sky Blue</t>
   </si>
   <si>
     <t>Sky Blue</t>
   </si>
   <si>
-    <t>52505-JEAN-DEN-SB-26</t>
-  </si>
-  <si>
-    <t>Jean BaggyDennis Reg. Cint. Sky Blue</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-SB-28</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-SB-30</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-SB-32</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-SB-34</t>
-  </si>
-  <si>
-    <t>Jean Baggy Dennis Reg. Cint. Wood Blue</t>
-  </si>
-  <si>
-    <t>Dennis Wood Blue</t>
-  </si>
-  <si>
-    <t>Wood Blue</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-WB-26</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-WB-28</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-WB-30</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-WB-32</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-WB-34</t>
-  </si>
-  <si>
-    <t>Jean Baggy Dennis Reg. Cint. Acid Wash</t>
-  </si>
-  <si>
-    <t>Dennis Acid Wash</t>
-  </si>
-  <si>
-    <t>Acid Wash</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-AW-26</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-AW-28</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-AW-30</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-AW-32</t>
-  </si>
-  <si>
-    <t>52505-JEAN-DEN-AW-34</t>
+    <t>601457549992</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-SB-26</t>
+  </si>
+  <si>
+    <t>603592062350</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-SB-28</t>
+  </si>
+  <si>
+    <t>603886898474</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-SB-30</t>
+  </si>
+  <si>
+    <t>602710365276</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-SB-32</t>
+  </si>
+  <si>
+    <t>604222587791</t>
+  </si>
+  <si>
+    <t>0625-JEAN-ROM-SB-34</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
   </si>
 </sst>
 </file>
@@ -245,6 +435,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,17 +473,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -590,19 +811,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H7" sqref="H7:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="13" max="13" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="13" max="13" width="55.83203125" customWidth="1"/>
+    <col min="14" max="14" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -707,17 +927,17 @@
       <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="2">
-        <v>602783942271</v>
+      <c r="M2" t="s">
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R2">
         <v>100</v>
@@ -729,7 +949,7 @@
         <v>95</v>
       </c>
       <c r="U2">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -740,7 +960,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -769,17 +989,17 @@
       <c r="L3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2">
-        <v>603665056981</v>
+      <c r="M3" t="s">
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P3">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R3">
         <v>100</v>
@@ -791,7 +1011,7 @@
         <v>95</v>
       </c>
       <c r="U3">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -802,13 +1022,13 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -831,17 +1051,17 @@
       <c r="L4" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="2">
-        <v>600792853872</v>
+      <c r="M4" t="s">
+        <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R4">
         <v>100</v>
@@ -853,7 +1073,7 @@
         <v>95</v>
       </c>
       <c r="U4">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -864,13 +1084,13 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -893,14 +1113,14 @@
       <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="2">
-        <v>603234629446</v>
+      <c r="M5" t="s">
+        <v>43</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5">
         <v>22</v>
@@ -915,7 +1135,7 @@
         <v>95</v>
       </c>
       <c r="U5">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -926,13 +1146,13 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -955,17 +1175,17 @@
       <c r="L6" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="2">
-        <v>600158122850</v>
+      <c r="M6" t="s">
+        <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R6">
         <v>100</v>
@@ -977,7 +1197,7 @@
         <v>95</v>
       </c>
       <c r="U6">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -988,10 +1208,10 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -1003,7 +1223,7 @@
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
@@ -1017,17 +1237,17 @@
       <c r="L7" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="2">
-        <v>603980425028</v>
+      <c r="M7" t="s">
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R7">
         <v>100</v>
@@ -1039,7 +1259,7 @@
         <v>95</v>
       </c>
       <c r="U7">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1053,7 +1273,7 @@
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
@@ -1065,7 +1285,7 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="I8" t="s">
         <v>29</v>
@@ -1079,17 +1299,17 @@
       <c r="L8" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="2">
-        <v>603631959498</v>
+      <c r="M8" t="s">
+        <v>52</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P8">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R8">
         <v>100</v>
@@ -1101,7 +1321,7 @@
         <v>95</v>
       </c>
       <c r="U8">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -1112,13 +1332,13 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -1127,7 +1347,7 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="I9" t="s">
         <v>29</v>
@@ -1141,17 +1361,17 @@
       <c r="L9" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="2">
-        <v>601106538064</v>
+      <c r="M9" t="s">
+        <v>54</v>
       </c>
       <c r="N9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P9">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R9">
         <v>100</v>
@@ -1163,7 +1383,7 @@
         <v>95</v>
       </c>
       <c r="U9">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -1174,13 +1394,13 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
@@ -1189,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="I10" t="s">
         <v>29</v>
@@ -1203,14 +1423,14 @@
       <c r="L10" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="2">
-        <v>602843779049</v>
+      <c r="M10" t="s">
+        <v>56</v>
       </c>
       <c r="N10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P10">
         <v>22</v>
@@ -1225,7 +1445,7 @@
         <v>95</v>
       </c>
       <c r="U10">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1236,13 +1456,13 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
@@ -1251,7 +1471,7 @@
         <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="I11" t="s">
         <v>29</v>
@@ -1265,17 +1485,17 @@
       <c r="L11" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="2">
-        <v>601838378870</v>
+      <c r="M11" t="s">
+        <v>58</v>
       </c>
       <c r="N11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R11">
         <v>100</v>
@@ -1287,7 +1507,7 @@
         <v>95</v>
       </c>
       <c r="U11">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1298,10 +1518,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1313,7 +1533,7 @@
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
         <v>29</v>
@@ -1327,17 +1547,17 @@
       <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="2">
-        <v>602131458545</v>
+      <c r="M12" t="s">
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="O12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R12">
         <v>100</v>
@@ -1349,7 +1569,7 @@
         <v>95</v>
       </c>
       <c r="U12">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -1360,10 +1580,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
@@ -1375,7 +1595,7 @@
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
         <v>29</v>
@@ -1389,17 +1609,17 @@
       <c r="L13" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="2">
-        <v>602956435585</v>
+      <c r="M13" t="s">
+        <v>65</v>
       </c>
       <c r="N13" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="O13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P13">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R13">
         <v>100</v>
@@ -1411,7 +1631,7 @@
         <v>95</v>
       </c>
       <c r="U13">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -1422,13 +1642,13 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
@@ -1437,7 +1657,7 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
         <v>29</v>
@@ -1451,17 +1671,17 @@
       <c r="L14" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="2">
-        <v>601733247673</v>
+      <c r="M14" t="s">
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="O14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P14">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R14">
         <v>100</v>
@@ -1473,7 +1693,7 @@
         <v>95</v>
       </c>
       <c r="U14">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -1484,13 +1704,13 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
         <v>26</v>
@@ -1499,7 +1719,7 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
         <v>29</v>
@@ -1513,14 +1733,14 @@
       <c r="L15" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="2">
-        <v>600181857375</v>
+      <c r="M15" t="s">
+        <v>69</v>
       </c>
       <c r="N15" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="O15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P15">
         <v>22</v>
@@ -1535,7 +1755,7 @@
         <v>95</v>
       </c>
       <c r="U15">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -1546,13 +1766,13 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
         <v>26</v>
@@ -1561,7 +1781,7 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I16" t="s">
         <v>29</v>
@@ -1575,17 +1795,17 @@
       <c r="L16" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="2">
-        <v>602537391321</v>
+      <c r="M16" t="s">
+        <v>71</v>
       </c>
       <c r="N16" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="O16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P16">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R16">
         <v>100</v>
@@ -1597,7 +1817,7 @@
         <v>95</v>
       </c>
       <c r="U16">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -1608,10 +1828,10 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -1623,7 +1843,7 @@
         <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
         <v>29</v>
@@ -1637,17 +1857,17 @@
       <c r="L17" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="2">
-        <v>604155392228</v>
+      <c r="M17" t="s">
+        <v>76</v>
       </c>
       <c r="N17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="O17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R17">
         <v>100</v>
@@ -1659,7 +1879,7 @@
         <v>95</v>
       </c>
       <c r="U17">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -1670,10 +1890,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>36</v>
@@ -1685,7 +1905,7 @@
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
         <v>29</v>
@@ -1699,17 +1919,17 @@
       <c r="L18" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="2">
-        <v>602042358508</v>
+      <c r="M18" t="s">
+        <v>78</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P18">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R18">
         <v>100</v>
@@ -1721,7 +1941,7 @@
         <v>95</v>
       </c>
       <c r="U18">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -1732,13 +1952,13 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -1747,7 +1967,7 @@
         <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>29</v>
@@ -1761,17 +1981,17 @@
       <c r="L19" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="2">
-        <v>600646159462</v>
+      <c r="M19" t="s">
+        <v>80</v>
       </c>
       <c r="N19" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P19">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R19">
         <v>100</v>
@@ -1783,7 +2003,7 @@
         <v>95</v>
       </c>
       <c r="U19">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -1794,13 +2014,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
@@ -1809,7 +2029,7 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I20" t="s">
         <v>29</v>
@@ -1823,14 +2043,14 @@
       <c r="L20" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="2">
-        <v>600653780706</v>
+      <c r="M20" t="s">
+        <v>82</v>
       </c>
       <c r="N20" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="O20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P20">
         <v>22</v>
@@ -1845,7 +2065,7 @@
         <v>95</v>
       </c>
       <c r="U20">
-        <v>125</v>
+        <v>149.9</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -1856,13 +2076,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
@@ -1871,7 +2091,7 @@
         <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
         <v>29</v>
@@ -1885,17 +2105,17 @@
       <c r="L21" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="2">
-        <v>603680627959</v>
+      <c r="M21" t="s">
+        <v>84</v>
       </c>
       <c r="N21" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="O21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P21">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R21">
         <v>100</v>
@@ -1907,10 +2127,949 @@
         <v>95</v>
       </c>
       <c r="U21">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22">
+        <v>15</v>
+      </c>
+      <c r="R22">
+        <v>100</v>
+      </c>
+      <c r="S22">
+        <v>75</v>
+      </c>
+      <c r="T22">
+        <v>95</v>
+      </c>
+      <c r="U22">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" t="s">
+        <v>93</v>
+      </c>
+      <c r="N23" t="s">
+        <v>94</v>
+      </c>
+      <c r="O23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23">
+        <v>43</v>
+      </c>
+      <c r="R23">
+        <v>100</v>
+      </c>
+      <c r="S23">
+        <v>75</v>
+      </c>
+      <c r="T23">
+        <v>95</v>
+      </c>
+      <c r="U23">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" t="s">
+        <v>95</v>
+      </c>
+      <c r="N24" t="s">
+        <v>96</v>
+      </c>
+      <c r="O24" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24">
+        <v>43</v>
+      </c>
+      <c r="R24">
+        <v>100</v>
+      </c>
+      <c r="S24">
+        <v>75</v>
+      </c>
+      <c r="T24">
+        <v>95</v>
+      </c>
+      <c r="U24">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25">
+        <v>29</v>
+      </c>
+      <c r="R25">
+        <v>100</v>
+      </c>
+      <c r="S25">
+        <v>75</v>
+      </c>
+      <c r="T25">
+        <v>95</v>
+      </c>
+      <c r="U25">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" t="s">
+        <v>99</v>
+      </c>
+      <c r="N26" t="s">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="R26">
+        <v>100</v>
+      </c>
+      <c r="S26">
+        <v>75</v>
+      </c>
+      <c r="T26">
+        <v>95</v>
+      </c>
+      <c r="U26">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" t="s">
+        <v>104</v>
+      </c>
+      <c r="N27" t="s">
+        <v>105</v>
+      </c>
+      <c r="O27" t="s">
+        <v>35</v>
+      </c>
+      <c r="P27">
+        <v>15</v>
+      </c>
+      <c r="R27">
+        <v>100</v>
+      </c>
+      <c r="S27">
+        <v>75</v>
+      </c>
+      <c r="T27">
+        <v>95</v>
+      </c>
+      <c r="U27">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" t="s">
+        <v>106</v>
+      </c>
+      <c r="N28" t="s">
+        <v>107</v>
+      </c>
+      <c r="O28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28">
+        <v>43</v>
+      </c>
+      <c r="R28">
+        <v>100</v>
+      </c>
+      <c r="S28">
+        <v>75</v>
+      </c>
+      <c r="T28">
+        <v>95</v>
+      </c>
+      <c r="U28">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" t="s">
+        <v>31</v>
+      </c>
+      <c r="L29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M29" t="s">
+        <v>108</v>
+      </c>
+      <c r="N29" t="s">
+        <v>109</v>
+      </c>
+      <c r="O29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29">
+        <v>43</v>
+      </c>
+      <c r="R29">
+        <v>100</v>
+      </c>
+      <c r="S29">
+        <v>75</v>
+      </c>
+      <c r="T29">
+        <v>95</v>
+      </c>
+      <c r="U29">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M30" t="s">
+        <v>110</v>
+      </c>
+      <c r="N30" t="s">
+        <v>111</v>
+      </c>
+      <c r="O30" t="s">
+        <v>35</v>
+      </c>
+      <c r="P30">
+        <v>29</v>
+      </c>
+      <c r="R30">
+        <v>100</v>
+      </c>
+      <c r="S30">
+        <v>75</v>
+      </c>
+      <c r="T30">
+        <v>95</v>
+      </c>
+      <c r="U30">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I31" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" t="s">
+        <v>113</v>
+      </c>
+      <c r="O31" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31">
+        <v>15</v>
+      </c>
+      <c r="R31">
+        <v>100</v>
+      </c>
+      <c r="S31">
+        <v>75</v>
+      </c>
+      <c r="T31">
+        <v>95</v>
+      </c>
+      <c r="U31">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" t="s">
+        <v>117</v>
+      </c>
+      <c r="N32" t="s">
+        <v>118</v>
+      </c>
+      <c r="O32" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32">
+        <v>15</v>
+      </c>
+      <c r="R32">
+        <v>100</v>
+      </c>
+      <c r="S32">
+        <v>75</v>
+      </c>
+      <c r="T32">
+        <v>95</v>
+      </c>
+      <c r="U32">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" t="s">
+        <v>30</v>
+      </c>
+      <c r="K33" t="s">
+        <v>31</v>
+      </c>
+      <c r="L33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M33" t="s">
+        <v>119</v>
+      </c>
+      <c r="N33" t="s">
+        <v>120</v>
+      </c>
+      <c r="O33" t="s">
+        <v>35</v>
+      </c>
+      <c r="P33">
+        <v>43</v>
+      </c>
+      <c r="R33">
+        <v>100</v>
+      </c>
+      <c r="S33">
+        <v>75</v>
+      </c>
+      <c r="T33">
+        <v>95</v>
+      </c>
+      <c r="U33">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" t="s">
+        <v>31</v>
+      </c>
+      <c r="L34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M34" t="s">
+        <v>121</v>
+      </c>
+      <c r="N34" t="s">
+        <v>122</v>
+      </c>
+      <c r="O34" t="s">
+        <v>35</v>
+      </c>
+      <c r="P34">
+        <v>43</v>
+      </c>
+      <c r="R34">
+        <v>100</v>
+      </c>
+      <c r="S34">
+        <v>75</v>
+      </c>
+      <c r="T34">
+        <v>95</v>
+      </c>
+      <c r="U34">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" t="s">
+        <v>116</v>
+      </c>
+      <c r="I35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M35" t="s">
+        <v>123</v>
+      </c>
+      <c r="N35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O35" t="s">
+        <v>35</v>
+      </c>
+      <c r="P35">
+        <v>29</v>
+      </c>
+      <c r="R35">
+        <v>100</v>
+      </c>
+      <c r="S35">
+        <v>75</v>
+      </c>
+      <c r="T35">
+        <v>95</v>
+      </c>
+      <c r="U35">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M36" t="s">
         <v>125</v>
       </c>
+      <c r="N36" t="s">
+        <v>126</v>
+      </c>
+      <c r="O36" t="s">
+        <v>35</v>
+      </c>
+      <c r="P36">
+        <v>15</v>
+      </c>
+      <c r="R36">
+        <v>100</v>
+      </c>
+      <c r="S36">
+        <v>75</v>
+      </c>
+      <c r="T36">
+        <v>95</v>
+      </c>
+      <c r="U36">
+        <v>149.9</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M1:M36">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M35">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N36">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update .DS_Store and productos.xlsx files
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13771373-F76F-614A-A82A-77F9D5262D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3699127-09E4-DE40-8A76-2E01632EA60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="56">
   <si>
     <t>Clasificación</t>
   </si>
@@ -116,34 +116,91 @@
     <t>Sí</t>
   </si>
   <si>
-    <t>Baggy</t>
-  </si>
-  <si>
     <t>Jeans</t>
   </si>
   <si>
-    <t>Cadera</t>
-  </si>
-  <si>
-    <t>Layer</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Wood Blue</t>
-  </si>
-  <si>
-    <t>Jean Baggy Layer Reg. Cad. Wood Blue</t>
-  </si>
-  <si>
-    <t>602705831349</t>
-  </si>
-  <si>
-    <t>52505-R-BAG-LAY-WB26</t>
-  </si>
-  <si>
-    <t>Baggy Layer Wood Blue</t>
+    <t>Fer Regular Corn Wash</t>
+  </si>
+  <si>
+    <t>Flare Fer Corn Wash</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Corn Wash</t>
+  </si>
+  <si>
+    <t>Fer</t>
+  </si>
+  <si>
+    <t>Cintura</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-CW-26</t>
+  </si>
+  <si>
+    <t>Talla 28</t>
+  </si>
+  <si>
+    <t>Talla 30</t>
+  </si>
+  <si>
+    <t>Talla 32</t>
+  </si>
+  <si>
+    <t>Talla 34</t>
+  </si>
+  <si>
+    <t>Fer Regular Green Blue</t>
+  </si>
+  <si>
+    <t>Flare Fer Green Blue</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-GB-26</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-GB-28</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-GB-30</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-GB-32</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-GB-34</t>
+  </si>
+  <si>
+    <t>Fer Regular Sky Blue</t>
+  </si>
+  <si>
+    <t>Flare Fer Sky Blue</t>
+  </si>
+  <si>
+    <t>Sky Blue</t>
+  </si>
+  <si>
+    <t>Green Blue</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-SB-26</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-SB-28</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-SB-30</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-SB-32</t>
+  </si>
+  <si>
+    <t>0625-FER-REG-SB-34</t>
   </si>
 </sst>
 </file>
@@ -173,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,12 +239,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,43 +279,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -261,9 +293,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,22 +631,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="27.6640625" customWidth="1"/>
-    <col min="13" max="13" width="55.83203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="30.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" customWidth="1"/>
     <col min="18" max="18" width="14.83203125" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" customWidth="1"/>
@@ -691,106 +724,916 @@
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5">
+        <v>100</v>
+      </c>
+      <c r="S2" s="5">
+        <v>75</v>
+      </c>
+      <c r="T2" s="5">
+        <v>95</v>
+      </c>
+      <c r="U2" s="5">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="5">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5">
+        <v>100</v>
+      </c>
+      <c r="S3" s="5">
+        <v>75</v>
+      </c>
+      <c r="T3" s="5">
+        <v>95</v>
+      </c>
+      <c r="U3" s="5">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="5">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5">
+        <v>100</v>
+      </c>
+      <c r="S4" s="5">
+        <v>75</v>
+      </c>
+      <c r="T4" s="5">
+        <v>95</v>
+      </c>
+      <c r="U4" s="5">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="5">
         <v>28</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
+        <v>100</v>
+      </c>
+      <c r="S5" s="5">
+        <v>75</v>
+      </c>
+      <c r="T5" s="5">
+        <v>95</v>
+      </c>
+      <c r="U5" s="5">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="J6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5">
+        <v>100</v>
+      </c>
+      <c r="S6" s="5">
+        <v>75</v>
+      </c>
+      <c r="T6" s="5">
+        <v>95</v>
+      </c>
+      <c r="U6" s="5">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="6">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6">
+        <v>100</v>
+      </c>
+      <c r="S7" s="6">
+        <v>75</v>
+      </c>
+      <c r="T7" s="6">
+        <v>95</v>
+      </c>
+      <c r="U7" s="6">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6">
+        <v>100</v>
+      </c>
+      <c r="S8" s="6">
+        <v>75</v>
+      </c>
+      <c r="T8" s="6">
+        <v>95</v>
+      </c>
+      <c r="U8" s="6">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6">
+        <v>100</v>
+      </c>
+      <c r="S9" s="6">
+        <v>75</v>
+      </c>
+      <c r="T9" s="6">
+        <v>95</v>
+      </c>
+      <c r="U9" s="6">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="6">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6">
+        <v>100</v>
+      </c>
+      <c r="S10" s="6">
+        <v>75</v>
+      </c>
+      <c r="T10" s="6">
+        <v>95</v>
+      </c>
+      <c r="U10" s="6">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="6">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
+        <v>100</v>
+      </c>
+      <c r="S11" s="6">
+        <v>75</v>
+      </c>
+      <c r="T11" s="6">
+        <v>95</v>
+      </c>
+      <c r="U11" s="6">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7">
+        <v>100</v>
+      </c>
+      <c r="S12" s="7">
+        <v>75</v>
+      </c>
+      <c r="T12" s="7">
+        <v>95</v>
+      </c>
+      <c r="U12" s="7">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M13" s="7"/>
+      <c r="N13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="7">
+        <v>40</v>
+      </c>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7">
+        <v>100</v>
+      </c>
+      <c r="S13" s="7">
+        <v>75</v>
+      </c>
+      <c r="T13" s="7">
+        <v>95</v>
+      </c>
+      <c r="U13" s="7">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="K14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6">
+      <c r="P14" s="7">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7">
         <v>100</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S14" s="7">
         <v>75</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T14" s="7">
         <v>95</v>
       </c>
-      <c r="U2" s="7">
+      <c r="U14" s="7">
         <v>149.9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M14"/>
-    </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M15"/>
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="7">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7">
+        <v>100</v>
+      </c>
+      <c r="S15" s="7">
+        <v>75</v>
+      </c>
+      <c r="T15" s="7">
+        <v>95</v>
+      </c>
+      <c r="U15" s="7">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M16"/>
+      <c r="A16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7">
+        <v>100</v>
+      </c>
+      <c r="S16" s="7">
+        <v>75</v>
+      </c>
+      <c r="T16" s="7">
+        <v>95</v>
+      </c>
+      <c r="U16" s="7">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M17"/>
@@ -825,7 +1668,7 @@
     <row r="46" spans="13:22" x14ac:dyDescent="0.2">
       <c r="M46"/>
       <c r="V46" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -834,17 +1677,17 @@
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="M51"/>
       <c r="V51" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M3:M33 M1">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="M17:M32">
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M32">
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
+  <conditionalFormatting sqref="M17:M33 M1">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N33">
+  <conditionalFormatting sqref="N17:N33">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update .DS_Store and productos.xlsx files; remove temporary Excel file
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D419FA35-31FD-6B4E-880E-6F046FFEB91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358E73D-706A-F24B-A444-5EF340DF2990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="140">
   <si>
     <t>Clasificación</t>
   </si>
@@ -439,10 +452,7 @@
     <t>0625-JEAN-SAM-PC-32</t>
   </si>
   <si>
-    <t>Casaca</t>
-  </si>
-  <si>
-    <t>Pantalón Baggy</t>
+    <t>Baggy</t>
   </si>
 </sst>
 </file>
@@ -809,11 +819,13 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E34" sqref="E34:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="13" max="13" width="48.33203125" customWidth="1"/>
   </cols>
@@ -899,9 +911,6 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
-        <v>139</v>
-      </c>
       <c r="H2" t="s">
         <v>26</v>
       </c>
@@ -955,9 +964,6 @@
       <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
-        <v>139</v>
-      </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
@@ -1011,9 +1017,6 @@
       <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
-        <v>139</v>
-      </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
@@ -1067,9 +1070,6 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
-        <v>139</v>
-      </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
@@ -1123,9 +1123,6 @@
       <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>139</v>
-      </c>
       <c r="H6" t="s">
         <v>44</v>
       </c>
@@ -1179,9 +1176,6 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
-        <v>139</v>
-      </c>
       <c r="H7" t="s">
         <v>44</v>
       </c>
@@ -1235,9 +1229,6 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" t="s">
-        <v>139</v>
-      </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
@@ -1291,9 +1282,6 @@
       <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
-        <v>139</v>
-      </c>
       <c r="H9" t="s">
         <v>44</v>
       </c>
@@ -1347,9 +1335,6 @@
       <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" t="s">
-        <v>139</v>
-      </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
@@ -1403,9 +1388,6 @@
       <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="G11" t="s">
-        <v>139</v>
-      </c>
       <c r="H11" t="s">
         <v>55</v>
       </c>
@@ -1459,9 +1441,6 @@
       <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="G12" t="s">
-        <v>139</v>
-      </c>
       <c r="H12" t="s">
         <v>55</v>
       </c>
@@ -1515,9 +1494,6 @@
       <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" t="s">
-        <v>139</v>
-      </c>
       <c r="H13" t="s">
         <v>55</v>
       </c>
@@ -1571,9 +1547,6 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
-        <v>139</v>
-      </c>
       <c r="H14" t="s">
         <v>66</v>
       </c>
@@ -1627,9 +1600,6 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="G15" t="s">
-        <v>139</v>
-      </c>
       <c r="H15" t="s">
         <v>66</v>
       </c>
@@ -1683,9 +1653,6 @@
       <c r="E16" t="s">
         <v>36</v>
       </c>
-      <c r="G16" t="s">
-        <v>139</v>
-      </c>
       <c r="H16" t="s">
         <v>66</v>
       </c>
@@ -1739,9 +1706,6 @@
       <c r="E17" t="s">
         <v>39</v>
       </c>
-      <c r="G17" t="s">
-        <v>139</v>
-      </c>
       <c r="H17" t="s">
         <v>66</v>
       </c>
@@ -1795,9 +1759,6 @@
       <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="G18" t="s">
-        <v>139</v>
-      </c>
       <c r="H18" t="s">
         <v>78</v>
       </c>
@@ -1851,9 +1812,6 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="G19" t="s">
-        <v>139</v>
-      </c>
       <c r="H19" t="s">
         <v>78</v>
       </c>
@@ -1907,9 +1865,6 @@
       <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="G20" t="s">
-        <v>139</v>
-      </c>
       <c r="H20" t="s">
         <v>78</v>
       </c>
@@ -1963,9 +1918,6 @@
       <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="G21" t="s">
-        <v>139</v>
-      </c>
       <c r="H21" t="s">
         <v>78</v>
       </c>
@@ -2019,9 +1971,6 @@
       <c r="E22" t="s">
         <v>25</v>
       </c>
-      <c r="G22" t="s">
-        <v>139</v>
-      </c>
       <c r="H22" t="s">
         <v>89</v>
       </c>
@@ -2075,9 +2024,6 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="G23" t="s">
-        <v>139</v>
-      </c>
       <c r="H23" t="s">
         <v>89</v>
       </c>
@@ -2131,9 +2077,6 @@
       <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="G24" t="s">
-        <v>139</v>
-      </c>
       <c r="H24" t="s">
         <v>89</v>
       </c>
@@ -2187,9 +2130,6 @@
       <c r="E25" t="s">
         <v>39</v>
       </c>
-      <c r="G25" t="s">
-        <v>139</v>
-      </c>
       <c r="H25" t="s">
         <v>89</v>
       </c>
@@ -2247,7 +2187,7 @@
         <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H26" t="s">
         <v>103</v>
@@ -2309,7 +2249,7 @@
         <v>102</v>
       </c>
       <c r="G27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H27" t="s">
         <v>103</v>
@@ -2371,7 +2311,7 @@
         <v>102</v>
       </c>
       <c r="G28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H28" t="s">
         <v>103</v>
@@ -2433,7 +2373,7 @@
         <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H29" t="s">
         <v>103</v>
@@ -2495,7 +2435,7 @@
         <v>102</v>
       </c>
       <c r="G30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H30" t="s">
         <v>119</v>
@@ -2557,7 +2497,7 @@
         <v>102</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H31" t="s">
         <v>119</v>
@@ -2619,7 +2559,7 @@
         <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H32" t="s">
         <v>119</v>
@@ -2681,7 +2621,7 @@
         <v>102</v>
       </c>
       <c r="G33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H33" t="s">
         <v>119</v>
@@ -2743,7 +2683,7 @@
         <v>102</v>
       </c>
       <c r="G34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H34" t="s">
         <v>130</v>
@@ -2805,7 +2745,7 @@
         <v>102</v>
       </c>
       <c r="G35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H35" t="s">
         <v>130</v>
@@ -2867,7 +2807,7 @@
         <v>102</v>
       </c>
       <c r="G36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H36" t="s">
         <v>130</v>
@@ -2929,7 +2869,7 @@
         <v>102</v>
       </c>
       <c r="G37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H37" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Add new Excel file with product codes and details for September 2025
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358E73D-706A-F24B-A444-5EF340DF2990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E04B9D-1F8C-CB4A-86DF-A3355D911C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="114">
   <si>
     <t>Clasificación</t>
   </si>
@@ -101,358 +101,280 @@
     <t>Producto</t>
   </si>
   <si>
-    <t>Casacas</t>
-  </si>
-  <si>
-    <t>Casaca Nikita Corn Wash</t>
-  </si>
-  <si>
-    <t>Nikita Corn Wash</t>
-  </si>
-  <si>
-    <t>Talla XS</t>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>Gaby Reg. Blue Green</t>
+  </si>
+  <si>
+    <t>Gaby Blue Green</t>
+  </si>
+  <si>
+    <t>Talla 26</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Blue Green</t>
+  </si>
+  <si>
+    <t>Gaby</t>
+  </si>
+  <si>
+    <t>Cintura</t>
+  </si>
+  <si>
+    <t>JOLG</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>601255216136</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-BG-26</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Talla 28</t>
+  </si>
+  <si>
+    <t>600246881407</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-BG-28</t>
+  </si>
+  <si>
+    <t>Talla 30</t>
+  </si>
+  <si>
+    <t>603898358457</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-BG-30</t>
+  </si>
+  <si>
+    <t>Talla 32</t>
+  </si>
+  <si>
+    <t>602034629950</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-BG-32</t>
+  </si>
+  <si>
+    <t>Talla 34</t>
+  </si>
+  <si>
+    <t>603901351399</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-BG-34</t>
+  </si>
+  <si>
+    <t>Gaby Reg. Light Brown</t>
+  </si>
+  <si>
+    <t>Gaby Light Brown</t>
+  </si>
+  <si>
+    <t>Light Brown</t>
+  </si>
+  <si>
+    <t>601554156444</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-LB-26</t>
+  </si>
+  <si>
+    <t>603753391276</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-LB-28</t>
+  </si>
+  <si>
+    <t>602806917134</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-LB-30</t>
+  </si>
+  <si>
+    <t>602439832462</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-LB-32</t>
+  </si>
+  <si>
+    <t>600476805585</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-LB-34</t>
+  </si>
+  <si>
+    <t>Gaby Reg. Sky Blue</t>
+  </si>
+  <si>
+    <t>Gaby Sky Blue</t>
+  </si>
+  <si>
+    <t>Sky Blue</t>
+  </si>
+  <si>
+    <t>600382886022</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-SB-26</t>
+  </si>
+  <si>
+    <t>603405446688</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-SB-28</t>
+  </si>
+  <si>
+    <t>603799843736</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-SB-30</t>
+  </si>
+  <si>
+    <t>600597116170</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-SB-32</t>
+  </si>
+  <si>
+    <t>601865132768</t>
+  </si>
+  <si>
+    <t>0625-JEAN-GAB-SB-34</t>
+  </si>
+  <si>
+    <t>Layci Reg. Corn Wash</t>
+  </si>
+  <si>
+    <t>Layci Corn Wash</t>
   </si>
   <si>
     <t>Corn Wash</t>
   </si>
   <si>
-    <t>Nikita</t>
-  </si>
-  <si>
-    <t>JOLG</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>600653809435</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-CW-XS</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>Talla S</t>
-  </si>
-  <si>
-    <t>601312239012</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-CW-S</t>
-  </si>
-  <si>
-    <t>Talla M</t>
-  </si>
-  <si>
-    <t>603397103400</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-CW-M</t>
-  </si>
-  <si>
-    <t>Talla L</t>
-  </si>
-  <si>
-    <t>603045047110</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-CW-L</t>
-  </si>
-  <si>
-    <t>Casaca Nikita Acid Wash</t>
-  </si>
-  <si>
-    <t>Nikita Acid Wash</t>
-  </si>
-  <si>
-    <t>Acid Wash</t>
-  </si>
-  <si>
-    <t>603111501470</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-AW-XS</t>
-  </si>
-  <si>
-    <t>603925599688</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-AW-S</t>
-  </si>
-  <si>
-    <t>601017114382</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-AW-M</t>
-  </si>
-  <si>
-    <t>600700468130</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-AW-L</t>
-  </si>
-  <si>
-    <t>Casaca Nikita Ice Wash</t>
-  </si>
-  <si>
-    <t>Nikita Ice Wash</t>
-  </si>
-  <si>
-    <t>Ice Wash</t>
-  </si>
-  <si>
-    <t>601235196904</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-IW-XS</t>
-  </si>
-  <si>
-    <t>603305630293</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-IW-S</t>
-  </si>
-  <si>
-    <t>602352659629</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-IW-M</t>
-  </si>
-  <si>
-    <t>603189226084</t>
-  </si>
-  <si>
-    <t>0625-CAS-NIK-IW-L</t>
-  </si>
-  <si>
-    <t>Casaca Miami Sky Blue</t>
-  </si>
-  <si>
-    <t>Miami Sky Blue</t>
-  </si>
-  <si>
-    <t>Sky Blue</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>602711921011</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-SB-XS</t>
-  </si>
-  <si>
-    <t>603543565819</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-SB-S</t>
-  </si>
-  <si>
-    <t>602336128278</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-SB-M</t>
-  </si>
-  <si>
-    <t>603052089311</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-SB-L</t>
-  </si>
-  <si>
-    <t>Casaca Miami Green Wash</t>
-  </si>
-  <si>
-    <t>Miami Green Wash</t>
-  </si>
-  <si>
-    <t>Green Wash</t>
-  </si>
-  <si>
-    <t>600034771446</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-GW-XS</t>
-  </si>
-  <si>
-    <t>600764894752</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-GW-S</t>
-  </si>
-  <si>
-    <t>600958028051</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-GW-M</t>
-  </si>
-  <si>
-    <t>601947398785</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-GW-L</t>
-  </si>
-  <si>
-    <t>Casaca Miami Brown Wash</t>
-  </si>
-  <si>
-    <t>Miami Brown Wash</t>
-  </si>
-  <si>
-    <t>Brown Wash</t>
-  </si>
-  <si>
-    <t>602214826597</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-BW-XS</t>
-  </si>
-  <si>
-    <t>601536520499</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-BW-S</t>
-  </si>
-  <si>
-    <t>603272843898</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-BW-M</t>
-  </si>
-  <si>
-    <t>602808357071</t>
-  </si>
-  <si>
-    <t>0625-CAS-MIA-BW-L</t>
-  </si>
-  <si>
-    <t>Jeans</t>
-  </si>
-  <si>
-    <t>Samantha Reg. Negro Crom.</t>
-  </si>
-  <si>
-    <t>Samantha Negro Crom.</t>
-  </si>
-  <si>
-    <t>Talla 26</t>
-  </si>
-  <si>
-    <t>Regular</t>
-  </si>
-  <si>
-    <t>Negro Cromado</t>
-  </si>
-  <si>
-    <t>Samantha</t>
-  </si>
-  <si>
-    <t>Cadera</t>
-  </si>
-  <si>
-    <t>603585871665</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-NC-26</t>
-  </si>
-  <si>
-    <t>Talla 28</t>
-  </si>
-  <si>
-    <t>603101695163</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-NC-28</t>
-  </si>
-  <si>
-    <t>Talla 30</t>
-  </si>
-  <si>
-    <t>601990807001</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-NC-30</t>
-  </si>
-  <si>
-    <t>Talla 32</t>
-  </si>
-  <si>
-    <t>603607544088</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-NC-32</t>
-  </si>
-  <si>
-    <t>Samantha Reg. Plomo Int.</t>
-  </si>
-  <si>
-    <t>Samantha Plomo Int.</t>
-  </si>
-  <si>
-    <t>Plomo Intermedio</t>
-  </si>
-  <si>
-    <t>604097044275</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PI-26</t>
-  </si>
-  <si>
-    <t>603935562367</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PI-28</t>
-  </si>
-  <si>
-    <t>602972330501</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PI-30</t>
-  </si>
-  <si>
-    <t>602730770108</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PI-32</t>
-  </si>
-  <si>
-    <t>Samantha Reg. Plomo Cen.</t>
-  </si>
-  <si>
-    <t>Samantha Plomo Cen.</t>
-  </si>
-  <si>
-    <t>Plomo Cenizo</t>
-  </si>
-  <si>
-    <t>604019890016</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PC-26</t>
-  </si>
-  <si>
-    <t>601792170516</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PC-28</t>
-  </si>
-  <si>
-    <t>600524872757</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PC-30</t>
-  </si>
-  <si>
-    <t>603905630916</t>
-  </si>
-  <si>
-    <t>0625-JEAN-SAM-PC-32</t>
-  </si>
-  <si>
-    <t>Baggy</t>
+    <t>Layci</t>
+  </si>
+  <si>
+    <t>600857880367</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-CW-26</t>
+  </si>
+  <si>
+    <t>602999943640</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-CW-28</t>
+  </si>
+  <si>
+    <t>600590894968</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-CW-30</t>
+  </si>
+  <si>
+    <t>600258886809</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-CW-32</t>
+  </si>
+  <si>
+    <t>601940294117</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-CW-34</t>
+  </si>
+  <si>
+    <t>Layci Reg. Light Blue</t>
+  </si>
+  <si>
+    <t>Layci Light Blue</t>
+  </si>
+  <si>
+    <t>Light Blue</t>
+  </si>
+  <si>
+    <t>600038872286</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-LB-26</t>
+  </si>
+  <si>
+    <t>602340387164</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-LB-28</t>
+  </si>
+  <si>
+    <t>602021499764</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-LB-30</t>
+  </si>
+  <si>
+    <t>603631535819</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-LB-32</t>
+  </si>
+  <si>
+    <t>601360630342</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-LB-34</t>
+  </si>
+  <si>
+    <t>Layci Reg. Wood Blue</t>
+  </si>
+  <si>
+    <t>Layci Wood Blue</t>
+  </si>
+  <si>
+    <t>Wood Blue</t>
+  </si>
+  <si>
+    <t>603834586738</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-WB-26</t>
+  </si>
+  <si>
+    <t>600981817372</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-WB-28</t>
+  </si>
+  <si>
+    <t>603943066932</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-WB-30</t>
+  </si>
+  <si>
+    <t>602745301553</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-WB-32</t>
+  </si>
+  <si>
+    <t>603323497558</t>
+  </si>
+  <si>
+    <t>0625-JEAN-LAY-WB-34</t>
+  </si>
+  <si>
+    <t>Pant. Semiflare</t>
   </si>
 </sst>
 </file>
@@ -816,18 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:E37"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="13" max="13" width="48.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -911,29 +831,38 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>113</v>
+      </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P2">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R2">
         <v>100</v>
@@ -962,31 +891,40 @@
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P3">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="R3">
         <v>100</v>
@@ -1015,31 +953,40 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>113</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P4">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="R4">
         <v>100</v>
@@ -1068,31 +1015,40 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P5">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R5">
         <v>100</v>
@@ -1115,25 +1071,34 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
         <v>45</v>
@@ -1142,10 +1107,10 @@
         <v>46</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P6">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R6">
         <v>100</v>
@@ -1168,37 +1133,46 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>113</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P7">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="R7">
         <v>100</v>
@@ -1221,37 +1195,46 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P8">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="R8">
         <v>100</v>
@@ -1274,37 +1257,46 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9">
         <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9">
-        <v>17</v>
       </c>
       <c r="R9">
         <v>100</v>
@@ -1327,25 +1319,34 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>113</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M10" t="s">
         <v>56</v>
@@ -1354,10 +1355,10 @@
         <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P10">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R10">
         <v>100</v>
@@ -1380,25 +1381,34 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>113</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M11" t="s">
         <v>58</v>
@@ -1407,10 +1417,10 @@
         <v>59</v>
       </c>
       <c r="O11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P11">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="R11">
         <v>100</v>
@@ -1433,37 +1443,46 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>113</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
       </c>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="O12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P12">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="R12">
         <v>100</v>
@@ -1486,37 +1505,46 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13">
         <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P13">
-        <v>17</v>
       </c>
       <c r="R13">
         <v>100</v>
@@ -1539,37 +1567,46 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" t="s">
         <v>67</v>
       </c>
-      <c r="K14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>68</v>
       </c>
-      <c r="N14" t="s">
-        <v>69</v>
-      </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P14">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="R14">
         <v>100</v>
@@ -1592,37 +1629,46 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M15" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" t="s">
         <v>70</v>
       </c>
-      <c r="N15" t="s">
-        <v>71</v>
-      </c>
       <c r="O15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P15">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R15">
         <v>100</v>
@@ -1645,37 +1691,46 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>28</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M16" t="s">
+        <v>71</v>
+      </c>
+      <c r="N16" t="s">
         <v>72</v>
       </c>
-      <c r="N16" t="s">
-        <v>73</v>
-      </c>
       <c r="O16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P16">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="R16">
         <v>100</v>
@@ -1698,37 +1753,46 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="J17" t="s">
+        <v>29</v>
       </c>
       <c r="K17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="N17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P17">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="R17">
         <v>100</v>
@@ -1751,25 +1815,34 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" t="s">
         <v>76</v>
       </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" t="s">
-        <v>67</v>
+      <c r="J18" t="s">
+        <v>29</v>
       </c>
       <c r="K18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M18" t="s">
         <v>79</v>
@@ -1778,10 +1851,10 @@
         <v>80</v>
       </c>
       <c r="O18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P18">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="R18">
         <v>100</v>
@@ -1804,25 +1877,34 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" t="s">
-        <v>67</v>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
       <c r="K19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
         <v>81</v>
@@ -1831,10 +1913,10 @@
         <v>82</v>
       </c>
       <c r="O19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P19">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R19">
         <v>100</v>
@@ -1857,25 +1939,34 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
         <v>76</v>
       </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" t="s">
-        <v>67</v>
+      <c r="J20" t="s">
+        <v>29</v>
       </c>
       <c r="K20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M20" t="s">
         <v>83</v>
@@ -1884,10 +1975,10 @@
         <v>84</v>
       </c>
       <c r="O20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P20">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="R20">
         <v>100</v>
@@ -1910,25 +2001,34 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
         <v>76</v>
       </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" t="s">
-        <v>67</v>
+      <c r="J21" t="s">
+        <v>29</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M21" t="s">
         <v>85</v>
@@ -1937,10 +2037,10 @@
         <v>86</v>
       </c>
       <c r="O21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P21">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="R21">
         <v>100</v>
@@ -1971,17 +2071,26 @@
       <c r="E22" t="s">
         <v>25</v>
       </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
       <c r="H22" t="s">
         <v>89</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
       </c>
       <c r="K22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M22" t="s">
         <v>90</v>
@@ -1990,10 +2099,10 @@
         <v>91</v>
       </c>
       <c r="O22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R22">
         <v>100</v>
@@ -2022,19 +2131,28 @@
         <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>113</v>
       </c>
       <c r="H23" t="s">
         <v>89</v>
       </c>
       <c r="I23" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="J23" t="s">
+        <v>29</v>
       </c>
       <c r="K23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M23" t="s">
         <v>92</v>
@@ -2043,10 +2161,10 @@
         <v>93</v>
       </c>
       <c r="O23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P23">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R23">
         <v>100</v>
@@ -2075,19 +2193,28 @@
         <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>113</v>
       </c>
       <c r="H24" t="s">
         <v>89</v>
       </c>
       <c r="I24" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M24" t="s">
         <v>94</v>
@@ -2096,10 +2223,10 @@
         <v>95</v>
       </c>
       <c r="O24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P24">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R24">
         <v>100</v>
@@ -2128,19 +2255,28 @@
         <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>113</v>
       </c>
       <c r="H25" t="s">
         <v>89</v>
       </c>
       <c r="I25" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="J25" t="s">
+        <v>29</v>
       </c>
       <c r="K25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M25" t="s">
         <v>96</v>
@@ -2149,10 +2285,10 @@
         <v>97</v>
       </c>
       <c r="O25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P25">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="R25">
         <v>100</v>
@@ -2172,49 +2308,49 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="N26" t="s">
         <v>99</v>
       </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" t="s">
-        <v>139</v>
-      </c>
-      <c r="H26" t="s">
-        <v>103</v>
-      </c>
-      <c r="I26" t="s">
-        <v>104</v>
-      </c>
-      <c r="J26" t="s">
-        <v>105</v>
-      </c>
-      <c r="K26" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" t="s">
-        <v>106</v>
-      </c>
-      <c r="N26" t="s">
-        <v>107</v>
-      </c>
       <c r="O26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P26">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="R26">
         <v>100</v>
@@ -2234,49 +2370,49 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" t="s">
         <v>102</v>
       </c>
-      <c r="G27" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" t="s">
         <v>103</v>
       </c>
-      <c r="I27" t="s">
+      <c r="N27" t="s">
         <v>104</v>
       </c>
-      <c r="J27" t="s">
-        <v>105</v>
-      </c>
-      <c r="K27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" t="s">
-        <v>29</v>
-      </c>
-      <c r="M27" t="s">
-        <v>109</v>
-      </c>
-      <c r="N27" t="s">
-        <v>110</v>
-      </c>
       <c r="O27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P27">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="R27">
         <v>100</v>
@@ -2296,49 +2432,49 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" t="s">
         <v>102</v>
       </c>
-      <c r="G28" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" t="s">
-        <v>103</v>
-      </c>
       <c r="I28" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M28" t="s">
         <v>105</v>
       </c>
-      <c r="K28" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M28" t="s">
-        <v>112</v>
-      </c>
       <c r="N28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="O28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P28">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="R28">
         <v>100</v>
@@ -2358,49 +2494,49 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" t="s">
         <v>102</v>
       </c>
-      <c r="G29" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" t="s">
-        <v>103</v>
-      </c>
       <c r="I29" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="J29" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M29" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="N29" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="O29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P29">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R29">
         <v>100</v>
@@ -2420,49 +2556,49 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" t="s">
         <v>102</v>
       </c>
-      <c r="G30" t="s">
-        <v>139</v>
-      </c>
-      <c r="H30" t="s">
-        <v>119</v>
-      </c>
       <c r="I30" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="J30" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="K30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M30" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="N30" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="O30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P30">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R30">
         <v>100</v>
@@ -2482,49 +2618,49 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" t="s">
         <v>102</v>
       </c>
-      <c r="G31" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" t="s">
-        <v>119</v>
-      </c>
       <c r="I31" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="J31" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="K31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M31" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="N31" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="O31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P31">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="R31">
         <v>100</v>
@@ -2536,378 +2672,6 @@
         <v>95</v>
       </c>
       <c r="U31">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" t="s">
-        <v>139</v>
-      </c>
-      <c r="H32" t="s">
-        <v>119</v>
-      </c>
-      <c r="I32" t="s">
-        <v>104</v>
-      </c>
-      <c r="J32" t="s">
-        <v>105</v>
-      </c>
-      <c r="K32" t="s">
-        <v>28</v>
-      </c>
-      <c r="L32" t="s">
-        <v>29</v>
-      </c>
-      <c r="M32" t="s">
-        <v>124</v>
-      </c>
-      <c r="N32" t="s">
-        <v>125</v>
-      </c>
-      <c r="O32" t="s">
-        <v>32</v>
-      </c>
-      <c r="P32">
-        <v>57</v>
-      </c>
-      <c r="R32">
-        <v>100</v>
-      </c>
-      <c r="S32">
-        <v>75</v>
-      </c>
-      <c r="T32">
-        <v>95</v>
-      </c>
-      <c r="U32">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" t="s">
-        <v>139</v>
-      </c>
-      <c r="H33" t="s">
-        <v>119</v>
-      </c>
-      <c r="I33" t="s">
-        <v>104</v>
-      </c>
-      <c r="J33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K33" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" t="s">
-        <v>29</v>
-      </c>
-      <c r="M33" t="s">
-        <v>126</v>
-      </c>
-      <c r="N33" t="s">
-        <v>127</v>
-      </c>
-      <c r="O33" t="s">
-        <v>32</v>
-      </c>
-      <c r="P33">
-        <v>30</v>
-      </c>
-      <c r="R33">
-        <v>100</v>
-      </c>
-      <c r="S33">
-        <v>75</v>
-      </c>
-      <c r="T33">
-        <v>95</v>
-      </c>
-      <c r="U33">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" t="s">
-        <v>102</v>
-      </c>
-      <c r="G34" t="s">
-        <v>139</v>
-      </c>
-      <c r="H34" t="s">
-        <v>130</v>
-      </c>
-      <c r="I34" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" t="s">
-        <v>105</v>
-      </c>
-      <c r="K34" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" t="s">
-        <v>29</v>
-      </c>
-      <c r="M34" t="s">
-        <v>131</v>
-      </c>
-      <c r="N34" t="s">
-        <v>132</v>
-      </c>
-      <c r="O34" t="s">
-        <v>32</v>
-      </c>
-      <c r="P34">
-        <v>30</v>
-      </c>
-      <c r="R34">
-        <v>100</v>
-      </c>
-      <c r="S34">
-        <v>75</v>
-      </c>
-      <c r="T34">
-        <v>95</v>
-      </c>
-      <c r="U34">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G35" t="s">
-        <v>139</v>
-      </c>
-      <c r="H35" t="s">
-        <v>130</v>
-      </c>
-      <c r="I35" t="s">
-        <v>104</v>
-      </c>
-      <c r="J35" t="s">
-        <v>105</v>
-      </c>
-      <c r="K35" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" t="s">
-        <v>29</v>
-      </c>
-      <c r="M35" t="s">
-        <v>133</v>
-      </c>
-      <c r="N35" t="s">
-        <v>134</v>
-      </c>
-      <c r="O35" t="s">
-        <v>32</v>
-      </c>
-      <c r="P35">
-        <v>57</v>
-      </c>
-      <c r="R35">
-        <v>100</v>
-      </c>
-      <c r="S35">
-        <v>75</v>
-      </c>
-      <c r="T35">
-        <v>95</v>
-      </c>
-      <c r="U35">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" t="s">
-        <v>111</v>
-      </c>
-      <c r="F36" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H36" t="s">
-        <v>130</v>
-      </c>
-      <c r="I36" t="s">
-        <v>104</v>
-      </c>
-      <c r="J36" t="s">
-        <v>105</v>
-      </c>
-      <c r="K36" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" t="s">
-        <v>29</v>
-      </c>
-      <c r="M36" t="s">
-        <v>135</v>
-      </c>
-      <c r="N36" t="s">
-        <v>136</v>
-      </c>
-      <c r="O36" t="s">
-        <v>32</v>
-      </c>
-      <c r="P36">
-        <v>57</v>
-      </c>
-      <c r="R36">
-        <v>100</v>
-      </c>
-      <c r="S36">
-        <v>75</v>
-      </c>
-      <c r="T36">
-        <v>95</v>
-      </c>
-      <c r="U36">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" t="s">
-        <v>102</v>
-      </c>
-      <c r="G37" t="s">
-        <v>139</v>
-      </c>
-      <c r="H37" t="s">
-        <v>130</v>
-      </c>
-      <c r="I37" t="s">
-        <v>104</v>
-      </c>
-      <c r="J37" t="s">
-        <v>105</v>
-      </c>
-      <c r="K37" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" t="s">
-        <v>29</v>
-      </c>
-      <c r="M37" t="s">
-        <v>137</v>
-      </c>
-      <c r="N37" t="s">
-        <v>138</v>
-      </c>
-      <c r="O37" t="s">
-        <v>32</v>
-      </c>
-      <c r="P37">
-        <v>30</v>
-      </c>
-      <c r="R37">
-        <v>100</v>
-      </c>
-      <c r="S37">
-        <v>75</v>
-      </c>
-      <c r="T37">
-        <v>95</v>
-      </c>
-      <c r="U37">
         <v>149.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Style: hide SKU in prints, remove borders, luxe B/W barcode
</commit_message>
<xml_diff>
--- a/data/productos.xlsx
+++ b/data/productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TRABAJO\jolg-etiquetas\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TRABAJO\oscarlorenzolima-etiquetas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AAFD4B-4ED7-40FD-84EC-5B184710FD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22326BC8-82AC-4F9D-B307-8EF989FF14F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,13 +508,19 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="34.7109375" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -646,5 +652,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>